<commit_message>
Cities names corr. in dataset
</commit_message>
<xml_diff>
--- a/migforecasting/cities11-12/1/d12.xlsx
+++ b/migforecasting/cities11-12/1/d12.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities11-12\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,9 +22,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="99">
   <si>
     <t>Балашиха</t>
-  </si>
-  <si>
-    <t>Домоде-дово</t>
   </si>
   <si>
     <t>Железнодорожный</t>
@@ -471,6 +468,9 @@
       </rPr>
       <t>6)</t>
     </r>
+  </si>
+  <si>
+    <t>Домодедово</t>
   </si>
 </sst>
 </file>
@@ -626,9 +626,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -640,6 +637,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="AA70" sqref="AA70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,61 +999,61 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
       <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>44</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>45</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>46</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>47</v>
-      </c>
-      <c r="V2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1126,49 +1126,49 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1176,69 +1176,69 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="12">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11">
         <v>235.3</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>104.7</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>141.69999999999999</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>106.9</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>144.69999999999999</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>187.3</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>127.6</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>181.1</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>178.7</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>101.8</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <v>137.80000000000001</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="11">
         <v>121.4</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="11">
         <v>206.7</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="11">
         <v>104.8</v>
       </c>
       <c r="Q5" s="5">
         <v>100.8</v>
       </c>
-      <c r="R5" s="12">
+      <c r="R5" s="11">
         <v>108.5</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="11">
         <v>126.8</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="11">
         <v>221.1</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="11">
         <v>113</v>
       </c>
-      <c r="V5" s="12">
+      <c r="V5" s="11">
         <v>156.6</v>
       </c>
-      <c r="W5" s="11"/>
+      <c r="W5" s="10"/>
       <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -1246,312 +1246,312 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="12">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
         <v>37</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>17.7</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>22.1</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>14</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11">
         <v>20.7</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>26.5</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>20.6</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>26.4</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>27.4</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>17.2</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>20</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="11">
         <v>18.8</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="11">
         <v>32</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="11">
         <v>15.7</v>
       </c>
       <c r="Q7" s="5">
         <v>15.2</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="11">
         <v>15.9</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="11">
         <v>18.8</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="11">
         <v>32.4</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="11">
         <v>18.100000000000001</v>
       </c>
-      <c r="V7" s="12">
+      <c r="V7" s="11">
         <v>21</v>
       </c>
-      <c r="W7" s="11"/>
+      <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="12">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11">
         <v>15.5</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>7.2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>9.1999999999999993</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>5.7</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <v>8.5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>10.7</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>9</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <v>10.7</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <v>11.3</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <v>6.9</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="11">
         <v>8.3000000000000007</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="11">
         <v>7.4</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="11">
         <v>12.8</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="11">
         <v>6.4</v>
       </c>
       <c r="Q8" s="5">
         <v>6.3</v>
       </c>
-      <c r="R8" s="12">
+      <c r="R8" s="11">
         <v>6.4</v>
       </c>
-      <c r="S8" s="12">
+      <c r="S8" s="11">
         <v>7.5</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8" s="11">
         <v>13.2</v>
       </c>
-      <c r="U8" s="12">
+      <c r="U8" s="11">
         <v>7.2</v>
       </c>
-      <c r="V8" s="12">
+      <c r="V8" s="11">
         <v>8.4</v>
       </c>
-      <c r="W8" s="11"/>
+      <c r="W8" s="10"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="12">
+        <v>14</v>
+      </c>
+      <c r="C9" s="11">
         <v>153.5</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>64.599999999999994</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>89.1</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>63.4</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <v>85.6</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>114</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>78.099999999999994</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <v>112.1</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>110.4</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <v>60.3</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="11">
         <v>86.2</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="11">
         <v>71.900000000000006</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="11">
         <v>124.8</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="11">
         <v>61.7</v>
       </c>
       <c r="Q9" s="5">
         <v>62</v>
       </c>
-      <c r="R9" s="12">
+      <c r="R9" s="11">
         <v>63.1</v>
       </c>
-      <c r="S9" s="12">
+      <c r="S9" s="11">
         <v>75.3</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="11">
         <v>138.30000000000001</v>
       </c>
-      <c r="U9" s="12">
+      <c r="U9" s="11">
         <v>67.7</v>
       </c>
-      <c r="V9" s="12">
+      <c r="V9" s="11">
         <v>95.7</v>
       </c>
-      <c r="W9" s="11"/>
+      <c r="W9" s="10"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="12">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11">
         <v>44.8</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>22.4</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>30.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>29.5</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>38.4</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <v>46.8</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="11">
         <v>28.9</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="11">
         <v>42.6</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <v>40.9</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="11">
         <v>24.3</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="11">
         <v>31.6</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="11">
         <v>30.7</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="11">
         <v>49.9</v>
       </c>
-      <c r="P10" s="12">
+      <c r="P10" s="11">
         <v>27.4</v>
       </c>
       <c r="Q10" s="5">
         <v>23.6</v>
       </c>
-      <c r="R10" s="12">
+      <c r="R10" s="11">
         <v>29.5</v>
       </c>
-      <c r="S10" s="12">
+      <c r="S10" s="11">
         <v>32.700000000000003</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="11">
         <v>50.4</v>
       </c>
-      <c r="U10" s="12">
+      <c r="U10" s="11">
         <v>27.2</v>
       </c>
-      <c r="V10" s="12">
+      <c r="V10" s="11">
         <v>39.9</v>
       </c>
-      <c r="W10" s="11"/>
+      <c r="W10" s="10"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5">
         <v>13.9</v>
@@ -1613,14 +1613,14 @@
       <c r="V11" s="5">
         <v>10.7</v>
       </c>
-      <c r="W11" s="11"/>
+      <c r="W11" s="10"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>11</v>
@@ -1682,14 +1682,14 @@
       <c r="V12" s="5">
         <v>14.2</v>
       </c>
-      <c r="W12" s="11"/>
+      <c r="W12" s="10"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <v>2.9</v>
@@ -1751,94 +1751,94 @@
       <c r="V13" s="5">
         <v>-3.5</v>
       </c>
-      <c r="W13" s="11"/>
+      <c r="W13" s="10"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="12">
+        <v>19</v>
+      </c>
+      <c r="C14" s="11">
         <v>12857</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>4219</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>5539</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>891</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <v>431</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>1939</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>4641</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <v>4616</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="11">
         <v>3620</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="11">
         <v>490</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="11">
         <v>146</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="11">
         <v>788</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="11">
         <v>13597</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="11">
         <v>1856</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="11">
         <v>1969</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="11">
         <v>-592</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="11">
         <v>897</v>
       </c>
-      <c r="T14" s="12">
+      <c r="T14" s="11">
         <v>5934</v>
       </c>
-      <c r="U14" s="12">
+      <c r="U14" s="11">
         <v>3103</v>
       </c>
-      <c r="V14" s="12">
+      <c r="V14" s="11">
         <v>1405</v>
       </c>
-      <c r="W14" s="11"/>
+      <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
@@ -1856,7 +1856,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5">
         <v>31.2</v>
@@ -1918,7 +1918,7 @@
       <c r="V16" s="5">
         <v>35.6</v>
       </c>
-      <c r="W16" s="11"/>
+      <c r="W16" s="10"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
     </row>
@@ -1927,10 +1927,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="5">
         <v>214</v>
@@ -1951,7 +1951,7 @@
         <v>212</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K17" s="5">
         <v>446</v>
@@ -1989,7 +1989,7 @@
       <c r="V17" s="5">
         <v>815</v>
       </c>
-      <c r="W17" s="11"/>
+      <c r="W17" s="10"/>
       <c r="X17" s="3"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -1997,7 +1997,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5">
         <v>590</v>
@@ -2059,83 +2059,83 @@
       <c r="V18" s="5">
         <v>594</v>
       </c>
-      <c r="W18" s="11"/>
+      <c r="W18" s="10"/>
     </row>
     <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="O19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="P19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="R19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="U19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="V19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="W19" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="V19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="W19" s="10"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5">
         <v>36291</v>
@@ -2197,14 +2197,14 @@
       <c r="V20" s="5">
         <v>30739</v>
       </c>
-      <c r="W20" s="11"/>
+      <c r="W20" s="10"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="5">
         <v>9770</v>
@@ -2266,7 +2266,7 @@
       <c r="V21" s="5">
         <v>10348</v>
       </c>
-      <c r="W21" s="11"/>
+      <c r="W21" s="10"/>
       <c r="X21" s="3"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="5">
         <v>45.2</v>
@@ -2298,7 +2298,7 @@
         <v>31.7</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K22" s="5">
         <v>48.4</v>
@@ -2336,7 +2336,7 @@
       <c r="V22" s="5">
         <v>45.5</v>
       </c>
-      <c r="W22" s="11"/>
+      <c r="W22" s="10"/>
       <c r="X22" s="3"/>
     </row>
     <row r="23" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5">
         <v>24.9</v>
@@ -2368,13 +2368,13 @@
         <v>31.1</v>
       </c>
       <c r="J23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="L23" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M23" s="5">
         <v>28.3</v>
@@ -2406,7 +2406,7 @@
       <c r="V23" s="5">
         <v>20.9</v>
       </c>
-      <c r="W23" s="11"/>
+      <c r="W23" s="10"/>
       <c r="X23" s="3"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2414,7 +2414,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="5">
         <v>44</v>
@@ -2476,14 +2476,14 @@
       <c r="V24" s="5">
         <v>43</v>
       </c>
-      <c r="W24" s="11"/>
+      <c r="W24" s="10"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -2494,7 +2494,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="12"/>
+      <c r="L25" s="11"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -2505,7 +2505,7 @@
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
-      <c r="W25" s="11"/>
+      <c r="W25" s="10"/>
       <c r="Y25" s="3"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -2513,7 +2513,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="5">
         <v>7.8</v>
@@ -2575,14 +2575,14 @@
       <c r="V26" s="5">
         <v>6</v>
       </c>
-      <c r="W26" s="11"/>
+      <c r="W26" s="10"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="5">
         <v>7.1</v>
@@ -2644,7 +2644,7 @@
       <c r="V27" s="5">
         <v>5.3</v>
       </c>
-      <c r="W27" s="11"/>
+      <c r="W27" s="10"/>
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -2652,36 +2652,36 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="5">
         <v>896</v>
@@ -2743,14 +2743,14 @@
       <c r="V29" s="5">
         <v>682</v>
       </c>
-      <c r="W29" s="11"/>
+      <c r="W29" s="10"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="5">
         <v>38.1</v>
@@ -2812,14 +2812,14 @@
       <c r="V30" s="5">
         <v>43.6</v>
       </c>
-      <c r="W30" s="11"/>
+      <c r="W30" s="10"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -2841,14 +2841,14 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
-      <c r="W31" s="11"/>
+      <c r="W31" s="10"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="5">
         <v>1424</v>
@@ -2910,7 +2910,7 @@
       <c r="V32" s="5">
         <v>1208</v>
       </c>
-      <c r="W32" s="11"/>
+      <c r="W32" s="10"/>
       <c r="X32" s="3"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -2918,7 +2918,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="5">
         <v>60.5</v>
@@ -2980,14 +2980,14 @@
       <c r="V33" s="5">
         <v>77.2</v>
       </c>
-      <c r="W33" s="11"/>
+      <c r="W33" s="10"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5">
         <v>6</v>
@@ -3049,7 +3049,7 @@
       <c r="V34" s="5">
         <v>16</v>
       </c>
-      <c r="W34" s="11"/>
+      <c r="W34" s="10"/>
       <c r="X34" s="4"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -3080,7 +3080,7 @@
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
-      <c r="W35" s="11"/>
+      <c r="W35" s="10"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -3088,7 +3088,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <v>2</v>
@@ -3150,7 +3150,7 @@
       <c r="V36" s="5">
         <v>1.4</v>
       </c>
-      <c r="W36" s="11"/>
+      <c r="W36" s="10"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -3158,7 +3158,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5">
         <v>84.1</v>
@@ -3220,7 +3220,7 @@
       <c r="V37" s="5">
         <v>92.4</v>
       </c>
-      <c r="W37" s="11"/>
+      <c r="W37" s="10"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
@@ -3228,7 +3228,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="5">
         <v>27</v>
@@ -3290,7 +3290,7 @@
       <c r="V38" s="5">
         <v>33</v>
       </c>
-      <c r="W38" s="11"/>
+      <c r="W38" s="10"/>
       <c r="Y38" s="3"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -3310,7 +3310,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="11"/>
+      <c r="L39" s="10"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
@@ -3321,7 +3321,7 @@
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
-      <c r="W39" s="11"/>
+      <c r="W39" s="10"/>
       <c r="Y39" s="3"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="5">
         <v>5.3</v>
@@ -3392,7 +3392,7 @@
       <c r="V40" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="W40" s="11"/>
+      <c r="W40" s="10"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -3400,7 +3400,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="5">
         <v>224.2</v>
@@ -3462,7 +3462,7 @@
       <c r="V41" s="5">
         <v>310.39999999999998</v>
       </c>
-      <c r="W41" s="11"/>
+      <c r="W41" s="10"/>
     </row>
     <row r="42" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -3470,10 +3470,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42" s="5">
         <v>2035</v>
@@ -3497,13 +3497,13 @@
         <v>5217</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L42" s="5">
         <v>1701</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N42" s="5">
         <v>2752</v>
@@ -3515,10 +3515,10 @@
         <v>786</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R42" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S42" s="5">
         <v>1645</v>
@@ -3532,7 +3532,7 @@
       <c r="V42" s="5">
         <v>1937</v>
       </c>
-      <c r="W42" s="11"/>
+      <c r="W42" s="10"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -3540,10 +3540,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43" s="5">
         <v>812</v>
@@ -3573,7 +3573,7 @@
         <v>593</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N43" s="5">
         <v>743</v>
@@ -3585,10 +3585,10 @@
         <v>326</v>
       </c>
       <c r="Q43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S43" s="5">
         <v>517</v>
@@ -3602,7 +3602,7 @@
       <c r="V43" s="5">
         <v>708</v>
       </c>
-      <c r="W43" s="11"/>
+      <c r="W43" s="10"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -3610,51 +3610,51 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="P44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="R44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="S44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="T44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="U44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="V44" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="W44" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="S44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="T44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="V44" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="W44" s="10"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -3662,7 +3662,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="5">
         <v>40240.400000000001</v>
@@ -3691,40 +3691,40 @@
       <c r="K45" s="5">
         <v>99668</v>
       </c>
-      <c r="L45" s="12">
+      <c r="L45" s="11">
         <v>85420.4</v>
       </c>
-      <c r="M45" s="12">
+      <c r="M45" s="11">
         <v>27285.7</v>
       </c>
-      <c r="N45" s="12">
+      <c r="N45" s="11">
         <v>17831.3</v>
       </c>
-      <c r="O45" s="12">
+      <c r="O45" s="11">
         <v>91250.6</v>
       </c>
-      <c r="P45" s="12">
+      <c r="P45" s="11">
         <v>15622.5</v>
       </c>
-      <c r="Q45" s="12">
+      <c r="Q45" s="11">
         <v>30057.5</v>
       </c>
-      <c r="R45" s="12">
+      <c r="R45" s="11">
         <v>22348.5</v>
       </c>
-      <c r="S45" s="12">
+      <c r="S45" s="11">
         <v>23777</v>
       </c>
-      <c r="T45" s="12">
+      <c r="T45" s="11">
         <v>168002</v>
       </c>
-      <c r="U45" s="12">
+      <c r="U45" s="11">
         <v>42864.4</v>
       </c>
-      <c r="V45" s="12">
+      <c r="V45" s="11">
         <v>44305.9</v>
       </c>
-      <c r="W45" s="11"/>
+      <c r="W45" s="10"/>
       <c r="Y45" s="3"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="5">
         <v>10080.4</v>
@@ -3762,40 +3762,40 @@
       <c r="K46" s="5">
         <v>16073.2</v>
       </c>
-      <c r="L46" s="12">
+      <c r="L46" s="11">
         <v>5140.5</v>
       </c>
-      <c r="M46" s="12">
+      <c r="M46" s="11">
         <v>3835.9</v>
       </c>
-      <c r="N46" s="12">
+      <c r="N46" s="11">
         <v>3040.4</v>
       </c>
-      <c r="O46" s="12">
+      <c r="O46" s="11">
         <v>17293</v>
       </c>
-      <c r="P46" s="12">
+      <c r="P46" s="11">
         <v>1905.2</v>
       </c>
-      <c r="Q46" s="12">
+      <c r="Q46" s="11">
         <v>3362.1</v>
       </c>
-      <c r="R46" s="12">
+      <c r="R46" s="11">
         <v>3971.8</v>
       </c>
-      <c r="S46" s="12">
+      <c r="S46" s="11">
         <v>3275.4</v>
       </c>
-      <c r="T46" s="12">
+      <c r="T46" s="11">
         <v>45248.4</v>
       </c>
-      <c r="U46" s="12">
+      <c r="U46" s="11">
         <v>3470.8</v>
       </c>
-      <c r="V46" s="12">
+      <c r="V46" s="11">
         <v>4578.6000000000004</v>
       </c>
-      <c r="W46" s="11"/>
+      <c r="W46" s="10"/>
       <c r="Y46" s="3"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
@@ -3804,7 +3804,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="5">
         <v>35.299999999999997</v>
@@ -3833,40 +3833,40 @@
       <c r="K47" s="5">
         <v>30.3</v>
       </c>
-      <c r="L47" s="12">
+      <c r="L47" s="11">
         <v>44.1</v>
       </c>
-      <c r="M47" s="12">
+      <c r="M47" s="11">
         <v>47.2</v>
       </c>
-      <c r="N47" s="12">
+      <c r="N47" s="11">
         <v>37.5</v>
       </c>
-      <c r="O47" s="12">
+      <c r="O47" s="11">
         <v>32</v>
       </c>
-      <c r="P47" s="12">
+      <c r="P47" s="11">
         <v>28.8</v>
       </c>
-      <c r="Q47" s="12">
+      <c r="Q47" s="11">
         <v>47.1</v>
       </c>
-      <c r="R47" s="12">
+      <c r="R47" s="11">
         <v>45.7</v>
       </c>
-      <c r="S47" s="12">
+      <c r="S47" s="11">
         <v>53.8</v>
       </c>
-      <c r="T47" s="12">
+      <c r="T47" s="11">
         <v>36.5</v>
       </c>
-      <c r="U47" s="12">
+      <c r="U47" s="11">
         <v>41.5</v>
       </c>
-      <c r="V47" s="12">
+      <c r="V47" s="11">
         <v>50.4</v>
       </c>
-      <c r="W47" s="11"/>
+      <c r="W47" s="10"/>
       <c r="Y47" s="3"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="5">
         <v>10</v>
@@ -3904,40 +3904,40 @@
       <c r="K48" s="5">
         <v>3.9</v>
       </c>
-      <c r="L48" s="12">
+      <c r="L48" s="11">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M48" s="12">
+      <c r="M48" s="11">
         <v>15.4</v>
       </c>
-      <c r="N48" s="12">
+      <c r="N48" s="11">
         <v>12.8</v>
       </c>
-      <c r="O48" s="12">
+      <c r="O48" s="11">
         <v>10.8</v>
       </c>
-      <c r="P48" s="12">
+      <c r="P48" s="11">
         <v>3.7</v>
       </c>
-      <c r="Q48" s="12">
+      <c r="Q48" s="11">
         <v>8.8000000000000007</v>
       </c>
-      <c r="R48" s="12">
+      <c r="R48" s="11">
         <v>17.8</v>
       </c>
-      <c r="S48" s="12">
+      <c r="S48" s="11">
         <v>14.6</v>
       </c>
-      <c r="T48" s="12">
+      <c r="T48" s="11">
         <v>7</v>
       </c>
-      <c r="U48" s="12">
+      <c r="U48" s="11">
         <v>13</v>
       </c>
-      <c r="V48" s="12">
+      <c r="V48" s="11">
         <v>20</v>
       </c>
-      <c r="W48" s="11"/>
+      <c r="W48" s="10"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -3945,51 +3945,51 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="N49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="P49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="R49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="S49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="T49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="U49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="V49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="W49" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="O49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="P49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="R49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="U49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="V49" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="W49" s="10"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -3997,7 +3997,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="5">
         <v>6053</v>
@@ -4026,40 +4026,40 @@
       <c r="K50" s="5">
         <v>11780</v>
       </c>
-      <c r="L50" s="11">
+      <c r="L50" s="10">
         <v>3275</v>
       </c>
-      <c r="M50" s="12">
+      <c r="M50" s="11">
         <v>8072</v>
       </c>
-      <c r="N50" s="12">
+      <c r="N50" s="11">
         <v>2068</v>
       </c>
-      <c r="O50" s="12">
+      <c r="O50" s="11">
         <v>8976</v>
       </c>
-      <c r="P50" s="12">
+      <c r="P50" s="11">
         <v>4516</v>
       </c>
-      <c r="Q50" s="12">
+      <c r="Q50" s="11">
         <v>3234</v>
       </c>
-      <c r="R50" s="12">
+      <c r="R50" s="11">
         <v>5246</v>
       </c>
-      <c r="S50" s="12">
+      <c r="S50" s="11">
         <v>3090</v>
       </c>
-      <c r="T50" s="12">
+      <c r="T50" s="11">
         <v>10156</v>
       </c>
-      <c r="U50" s="12">
+      <c r="U50" s="11">
         <v>4126</v>
       </c>
-      <c r="V50" s="12">
+      <c r="V50" s="11">
         <v>2865</v>
       </c>
-      <c r="W50" s="11"/>
+      <c r="W50" s="10"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -4067,29 +4067,29 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="10"/>
+      <c r="W51" s="10"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -4097,29 +4097,29 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10"/>
+      <c r="V52" s="10"/>
+      <c r="W52" s="10"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -4127,69 +4127,69 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G53" s="5">
         <v>3</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="M53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R53" s="12">
+        <v>65</v>
+      </c>
+      <c r="L53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R53" s="11">
         <v>1</v>
       </c>
-      <c r="S53" s="12">
+      <c r="S53" s="11">
         <v>1</v>
       </c>
-      <c r="T53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="U53" s="12">
+      <c r="T53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U53" s="11">
         <v>2</v>
       </c>
-      <c r="V53" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W53" s="11"/>
+      <c r="V53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W53" s="10"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
@@ -4197,7 +4197,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="5">
         <v>35</v>
@@ -4226,40 +4226,40 @@
       <c r="K54" s="5">
         <v>40</v>
       </c>
-      <c r="L54" s="12">
+      <c r="L54" s="11">
         <v>42</v>
       </c>
-      <c r="M54" s="12">
+      <c r="M54" s="11">
         <v>19</v>
       </c>
-      <c r="N54" s="12">
+      <c r="N54" s="11">
         <v>36</v>
       </c>
-      <c r="O54" s="12">
+      <c r="O54" s="11">
         <v>75</v>
       </c>
-      <c r="P54" s="12">
+      <c r="P54" s="11">
         <v>15</v>
       </c>
-      <c r="Q54" s="12">
+      <c r="Q54" s="11">
         <v>29</v>
       </c>
-      <c r="R54" s="12">
+      <c r="R54" s="11">
         <v>40</v>
       </c>
-      <c r="S54" s="12">
+      <c r="S54" s="11">
         <v>36</v>
       </c>
-      <c r="T54" s="12">
+      <c r="T54" s="11">
         <v>45</v>
       </c>
-      <c r="U54" s="12">
+      <c r="U54" s="11">
         <v>39</v>
       </c>
-      <c r="V54" s="12">
+      <c r="V54" s="11">
         <v>58</v>
       </c>
-      <c r="W54" s="11"/>
+      <c r="W54" s="10"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -4267,7 +4267,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="5">
         <v>7</v>
@@ -4296,40 +4296,40 @@
       <c r="K55" s="5">
         <v>14</v>
       </c>
-      <c r="L55" s="12">
+      <c r="L55" s="11">
         <v>12</v>
       </c>
-      <c r="M55" s="12">
+      <c r="M55" s="11">
         <v>9</v>
       </c>
-      <c r="N55" s="12">
+      <c r="N55" s="11">
         <v>8</v>
       </c>
-      <c r="O55" s="12">
+      <c r="O55" s="11">
         <v>18</v>
       </c>
-      <c r="P55" s="12">
+      <c r="P55" s="11">
         <v>6</v>
       </c>
-      <c r="Q55" s="12">
+      <c r="Q55" s="11">
         <v>11</v>
       </c>
-      <c r="R55" s="12">
+      <c r="R55" s="11">
         <v>12</v>
       </c>
-      <c r="S55" s="12">
+      <c r="S55" s="11">
         <v>10</v>
       </c>
-      <c r="T55" s="12">
+      <c r="T55" s="11">
         <v>13</v>
       </c>
-      <c r="U55" s="12">
+      <c r="U55" s="11">
         <v>9</v>
       </c>
-      <c r="V55" s="12">
+      <c r="V55" s="11">
         <v>14</v>
       </c>
-      <c r="W55" s="11"/>
+      <c r="W55" s="10"/>
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
@@ -4338,7 +4338,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -4349,18 +4349,18 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
-      <c r="W56" s="11"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="10"/>
       <c r="Y56" s="3"/>
     </row>
     <row r="57" spans="1:26" ht="17.25" x14ac:dyDescent="0.25">
@@ -4369,69 +4369,69 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G57" s="5">
         <v>205.2</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="M57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R57" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="S57" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="T57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="U57" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="V57" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W57" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="L57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="S57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="T57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="V57" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W57" s="10"/>
       <c r="Y57" s="3"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="5">
         <v>15769.8</v>
@@ -4469,40 +4469,40 @@
       <c r="K58" s="5">
         <v>64806.3</v>
       </c>
-      <c r="L58" s="12">
+      <c r="L58" s="11">
         <v>16030.1</v>
       </c>
-      <c r="M58" s="12">
+      <c r="M58" s="11">
         <v>17589.599999999999</v>
       </c>
-      <c r="N58" s="12">
+      <c r="N58" s="11">
         <v>8129.4</v>
       </c>
-      <c r="O58" s="12">
+      <c r="O58" s="11">
         <v>41191.9</v>
       </c>
-      <c r="P58" s="12">
+      <c r="P58" s="11">
         <v>9989.1</v>
       </c>
-      <c r="Q58" s="12">
+      <c r="Q58" s="11">
         <v>20774.400000000001</v>
       </c>
-      <c r="R58" s="12">
+      <c r="R58" s="11">
         <v>5464.3</v>
       </c>
-      <c r="S58" s="12">
+      <c r="S58" s="11">
         <v>13498.7</v>
       </c>
-      <c r="T58" s="12">
+      <c r="T58" s="11">
         <v>14921</v>
       </c>
-      <c r="U58" s="12">
+      <c r="U58" s="11">
         <v>63040.7</v>
       </c>
-      <c r="V58" s="12">
+      <c r="V58" s="11">
         <v>34383.199999999997</v>
       </c>
-      <c r="W58" s="11"/>
+      <c r="W58" s="10"/>
       <c r="Y58" s="3"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
@@ -4511,7 +4511,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="5">
         <v>4036.5</v>
@@ -4540,40 +4540,40 @@
       <c r="K59" s="5">
         <v>7766</v>
       </c>
-      <c r="L59" s="12">
+      <c r="L59" s="11">
         <v>18074</v>
       </c>
-      <c r="M59" s="12">
+      <c r="M59" s="11">
         <v>9911.6</v>
       </c>
-      <c r="N59" s="12">
+      <c r="N59" s="11">
         <v>1792.1</v>
       </c>
-      <c r="O59" s="12">
+      <c r="O59" s="11">
         <v>22545.599999999999</v>
       </c>
-      <c r="P59" s="12">
+      <c r="P59" s="11">
         <v>1614</v>
       </c>
-      <c r="Q59" s="12">
+      <c r="Q59" s="11">
         <v>4214.1000000000004</v>
       </c>
-      <c r="R59" s="12">
+      <c r="R59" s="11">
         <v>2083.5</v>
       </c>
-      <c r="S59" s="12">
+      <c r="S59" s="11">
         <v>2802</v>
       </c>
-      <c r="T59" s="12">
+      <c r="T59" s="11">
         <v>2363.6</v>
       </c>
-      <c r="U59" s="12">
+      <c r="U59" s="11">
         <v>2151</v>
       </c>
-      <c r="V59" s="12">
+      <c r="V59" s="11">
         <v>2439.1999999999998</v>
       </c>
-      <c r="W59" s="11"/>
+      <c r="W59" s="10"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
@@ -4581,31 +4581,31 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
-      <c r="O60" s="9"/>
-      <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
-      <c r="R60" s="9"/>
-      <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
-      <c r="V60" s="9"/>
-      <c r="W60" s="9"/>
+        <v>71</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M60" s="13"/>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13"/>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
+      <c r="T60" s="13"/>
+      <c r="U60" s="13"/>
+      <c r="V60" s="13"/>
+      <c r="W60" s="13"/>
     </row>
     <row r="61" spans="1:26" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -4613,7 +4613,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="5">
         <v>3479.2</v>
@@ -4642,40 +4642,40 @@
       <c r="K61" s="5">
         <v>8687.1</v>
       </c>
-      <c r="L61" s="12">
+      <c r="L61" s="11">
         <v>50.5</v>
       </c>
-      <c r="M61" s="12">
+      <c r="M61" s="11">
         <v>2160.8000000000002</v>
       </c>
-      <c r="N61" s="12">
+      <c r="N61" s="11">
         <v>2093.4</v>
       </c>
-      <c r="O61" s="12">
+      <c r="O61" s="11">
         <v>4118.3</v>
       </c>
-      <c r="P61" s="12">
+      <c r="P61" s="11">
         <v>196.9</v>
       </c>
-      <c r="Q61" s="12">
+      <c r="Q61" s="11">
         <v>4481.6000000000004</v>
       </c>
-      <c r="R61" s="12">
+      <c r="R61" s="11">
         <v>2901.7</v>
       </c>
-      <c r="S61" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="T61" s="12">
+      <c r="S61" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="T61" s="11">
         <v>3335.6</v>
       </c>
-      <c r="U61" s="12">
+      <c r="U61" s="11">
         <v>1272.5</v>
       </c>
-      <c r="V61" s="12">
+      <c r="V61" s="11">
         <v>869.7</v>
       </c>
-      <c r="W61" s="11"/>
+      <c r="W61" s="10"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -4683,7 +4683,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -4694,18 +4694,18 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="12"/>
-      <c r="S62" s="12"/>
-      <c r="T62" s="12"/>
-      <c r="U62" s="12"/>
-      <c r="V62" s="12"/>
-      <c r="W62" s="11"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="T62" s="11"/>
+      <c r="U62" s="11"/>
+      <c r="V62" s="11"/>
+      <c r="W62" s="10"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -4713,7 +4713,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="5">
         <v>422.7</v>
@@ -4742,40 +4742,40 @@
       <c r="K63" s="5">
         <v>366.9</v>
       </c>
-      <c r="L63" s="12">
+      <c r="L63" s="11">
         <v>14.2</v>
       </c>
-      <c r="M63" s="12">
+      <c r="M63" s="11">
         <v>141.1</v>
       </c>
-      <c r="N63" s="12">
+      <c r="N63" s="11">
         <v>4.8</v>
       </c>
-      <c r="O63" s="12">
+      <c r="O63" s="11">
         <v>200.4</v>
       </c>
-      <c r="P63" s="12">
+      <c r="P63" s="11">
         <v>125.7</v>
       </c>
-      <c r="Q63" s="12">
+      <c r="Q63" s="11">
         <v>104.6</v>
       </c>
-      <c r="R63" s="12">
+      <c r="R63" s="11">
         <v>57</v>
       </c>
-      <c r="S63" s="12">
+      <c r="S63" s="11">
         <v>81.3</v>
       </c>
-      <c r="T63" s="12">
+      <c r="T63" s="11">
         <v>343.1</v>
       </c>
-      <c r="U63" s="12">
+      <c r="U63" s="11">
         <v>129.1</v>
       </c>
-      <c r="V63" s="12">
+      <c r="V63" s="11">
         <v>10.199999999999999</v>
       </c>
-      <c r="W63" s="11"/>
+      <c r="W63" s="10"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -4783,7 +4783,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="5">
         <v>6395</v>
@@ -4812,40 +4812,40 @@
       <c r="K64" s="5">
         <v>4183</v>
       </c>
-      <c r="L64" s="12">
+      <c r="L64" s="11">
         <v>269</v>
       </c>
-      <c r="M64" s="12">
+      <c r="M64" s="11">
         <v>574</v>
       </c>
-      <c r="N64" s="12">
+      <c r="N64" s="11">
         <v>17</v>
       </c>
-      <c r="O64" s="12">
+      <c r="O64" s="11">
         <v>3081</v>
       </c>
-      <c r="P64" s="12">
+      <c r="P64" s="11">
         <v>1131</v>
       </c>
-      <c r="Q64" s="12">
+      <c r="Q64" s="11">
         <v>1601</v>
       </c>
-      <c r="R64" s="12">
+      <c r="R64" s="11">
         <v>757</v>
       </c>
-      <c r="S64" s="12">
+      <c r="S64" s="11">
         <v>1093</v>
       </c>
-      <c r="T64" s="12">
+      <c r="T64" s="11">
         <v>5479</v>
       </c>
-      <c r="U64" s="12">
+      <c r="U64" s="11">
         <v>2069</v>
       </c>
-      <c r="V64" s="12">
+      <c r="V64" s="11">
         <v>175</v>
       </c>
-      <c r="W64" s="11"/>
+      <c r="W64" s="10"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -4859,10 +4859,10 @@
         <v>120</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G65" s="5">
         <v>80</v>
@@ -4880,39 +4880,39 @@
         <v>325</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M65" s="12">
-        <v>65</v>
-      </c>
-      <c r="N65" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O65" s="12">
+        <v>65</v>
+      </c>
+      <c r="M65" s="11">
+        <v>65</v>
+      </c>
+      <c r="N65" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O65" s="11">
         <v>140</v>
       </c>
-      <c r="P65" s="12">
+      <c r="P65" s="11">
         <v>120</v>
       </c>
-      <c r="Q65" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R65" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S65" s="12">
+      <c r="Q65" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R65" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S65" s="11">
         <v>220</v>
       </c>
-      <c r="T65" s="12">
+      <c r="T65" s="11">
         <v>225</v>
       </c>
-      <c r="U65" s="12">
+      <c r="U65" s="11">
         <v>135</v>
       </c>
-      <c r="V65" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W65" s="11"/>
+      <c r="V65" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W65" s="10"/>
       <c r="Y65" s="3"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
@@ -4921,67 +4921,67 @@
         <v>64</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" s="5">
         <v>825</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I66" s="5">
         <v>982</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K66" s="5">
         <v>1000</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O66" s="12">
+        <v>65</v>
+      </c>
+      <c r="M66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O66" s="11">
         <v>2200</v>
       </c>
-      <c r="P66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q66" s="12">
+      <c r="P66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q66" s="11">
         <v>288</v>
       </c>
-      <c r="R66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="T66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="U66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V66" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W66" s="12"/>
-      <c r="Y66" s="10"/>
+      <c r="R66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V66" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W66" s="11"/>
+      <c r="Y66" s="9"/>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -4989,66 +4989,66 @@
         <v>65</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="T67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="U67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V67" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W67" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="M67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V67" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W67" s="11"/>
       <c r="X67" s="3"/>
       <c r="Y67" s="3"/>
     </row>
@@ -5058,68 +5058,68 @@
         <v>66</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="P68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="T68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="U68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V68" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="W68" s="11"/>
+        <v>65</v>
+      </c>
+      <c r="M68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="V68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="W68" s="10"/>
       <c r="X68" s="3"/>
-      <c r="Y68" s="10"/>
+      <c r="Y68" s="9"/>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -5127,29 +5127,29 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="12"/>
-      <c r="N69" s="12"/>
-      <c r="O69" s="12"/>
-      <c r="P69" s="12"/>
-      <c r="Q69" s="12"/>
-      <c r="R69" s="12"/>
-      <c r="S69" s="12"/>
-      <c r="T69" s="12"/>
-      <c r="U69" s="12"/>
-      <c r="V69" s="12"/>
-      <c r="W69" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="11"/>
+      <c r="U69" s="11"/>
+      <c r="V69" s="11"/>
+      <c r="W69" s="11"/>
       <c r="Y69" s="3"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
@@ -5158,33 +5158,33 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="12">
+        <v>81</v>
+      </c>
+      <c r="C70" s="11">
         <v>23304.6</v>
       </c>
-      <c r="D70" s="12">
+      <c r="D70" s="11">
         <v>17869.8</v>
       </c>
-      <c r="E70" s="12">
+      <c r="E70" s="11">
         <v>4564.8</v>
       </c>
-      <c r="F70" s="12">
+      <c r="F70" s="11">
         <v>5515.5</v>
       </c>
-      <c r="G70" s="12">
+      <c r="G70" s="11">
         <v>7187.5</v>
       </c>
-      <c r="H70" s="12">
+      <c r="H70" s="11">
         <v>13154.4</v>
       </c>
-      <c r="I70" s="12">
+      <c r="I70" s="11">
         <v>7058.8</v>
       </c>
-      <c r="J70" s="12">
+      <c r="J70" s="11">
         <v>13960.9</v>
       </c>
-      <c r="K70" s="12">
+      <c r="K70" s="11">
         <v>66362.600000000006</v>
       </c>
       <c r="L70" s="5">
@@ -5220,8 +5220,8 @@
       <c r="V70" s="5">
         <v>7612.1</v>
       </c>
-      <c r="W70" s="12"/>
-      <c r="Y70" s="10"/>
+      <c r="W70" s="11"/>
+      <c r="Y70" s="9"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -5229,33 +5229,33 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" s="12">
+        <v>82</v>
+      </c>
+      <c r="C71" s="11">
         <v>122.5</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D71" s="11">
         <v>103.4</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E71" s="11">
         <v>115.8</v>
       </c>
-      <c r="F71" s="12">
+      <c r="F71" s="11">
         <v>83.7</v>
       </c>
-      <c r="G71" s="12">
+      <c r="G71" s="11">
         <v>113</v>
       </c>
-      <c r="H71" s="12">
+      <c r="H71" s="11">
         <v>124.4</v>
       </c>
-      <c r="I71" s="12">
+      <c r="I71" s="11">
         <v>103.4</v>
       </c>
-      <c r="J71" s="12">
+      <c r="J71" s="11">
         <v>103.4</v>
       </c>
-      <c r="K71" s="12">
+      <c r="K71" s="11">
         <v>103.6</v>
       </c>
       <c r="L71" s="5">
@@ -5291,7 +5291,7 @@
       <c r="V71" s="5">
         <v>117.8</v>
       </c>
-      <c r="W71" s="12"/>
+      <c r="W71" s="11"/>
       <c r="Y71" s="3"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
@@ -5300,33 +5300,33 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="12">
+        <v>83</v>
+      </c>
+      <c r="C72" s="11">
         <v>858.4</v>
       </c>
-      <c r="D72" s="12">
+      <c r="D72" s="11">
         <v>6775.4</v>
       </c>
-      <c r="E72" s="12">
+      <c r="E72" s="11">
         <v>745.5</v>
       </c>
-      <c r="F72" s="12">
+      <c r="F72" s="11">
         <v>3.6</v>
       </c>
-      <c r="G72" s="12">
+      <c r="G72" s="11">
         <v>484.6</v>
       </c>
-      <c r="H72" s="12">
+      <c r="H72" s="11">
         <v>242</v>
       </c>
-      <c r="I72" s="12">
+      <c r="I72" s="11">
         <v>940</v>
       </c>
-      <c r="J72" s="12">
+      <c r="J72" s="11">
         <v>737.7</v>
       </c>
-      <c r="K72" s="12">
+      <c r="K72" s="11">
         <v>149.80000000000001</v>
       </c>
       <c r="L72" s="5">
@@ -5362,7 +5362,7 @@
       <c r="V72" s="5">
         <v>578.9</v>
       </c>
-      <c r="W72" s="12"/>
+      <c r="W72" s="11"/>
       <c r="Y72" s="3"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
@@ -5371,34 +5371,34 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="12">
+        <v>84</v>
+      </c>
+      <c r="C73" s="11">
         <v>151.19999999999999</v>
       </c>
-      <c r="D73" s="12">
+      <c r="D73" s="11">
         <v>99.9</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" s="11">
+        <v>134.9</v>
+      </c>
+      <c r="G73" s="11">
+        <v>116.2</v>
+      </c>
+      <c r="H73" s="11">
+        <v>109</v>
+      </c>
+      <c r="I73" s="11">
+        <v>127.9</v>
+      </c>
+      <c r="J73" s="11">
+        <v>142.1</v>
+      </c>
+      <c r="K73" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="F73" s="12">
-        <v>134.9</v>
-      </c>
-      <c r="G73" s="12">
-        <v>116.2</v>
-      </c>
-      <c r="H73" s="12">
-        <v>109</v>
-      </c>
-      <c r="I73" s="12">
-        <v>127.9</v>
-      </c>
-      <c r="J73" s="12">
-        <v>142.1</v>
-      </c>
-      <c r="K73" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="L73" s="5">
         <v>146.19999999999999</v>
@@ -5433,9 +5433,9 @@
       <c r="V73" s="5">
         <v>126.3</v>
       </c>
-      <c r="W73" s="11"/>
+      <c r="W73" s="10"/>
       <c r="X73" s="3"/>
-      <c r="Y73" s="10"/>
+      <c r="Y73" s="9"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
@@ -5443,28 +5443,28 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
-      <c r="T74" s="11"/>
-      <c r="U74" s="11"/>
-      <c r="V74" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
+      <c r="V74" s="10"/>
       <c r="W74" s="5"/>
       <c r="X74" s="3"/>
     </row>
@@ -5474,33 +5474,33 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
-      </c>
-      <c r="C75" s="12">
+        <v>85</v>
+      </c>
+      <c r="C75" s="11">
         <v>4762.8999999999996</v>
       </c>
-      <c r="D75" s="12">
+      <c r="D75" s="11">
         <v>14431.6</v>
       </c>
-      <c r="E75" s="12">
+      <c r="E75" s="11">
         <v>4596.6000000000004</v>
       </c>
-      <c r="F75" s="12">
+      <c r="F75" s="11">
         <v>1290</v>
       </c>
-      <c r="G75" s="12">
+      <c r="G75" s="11">
         <v>4583.8999999999996</v>
       </c>
-      <c r="H75" s="12">
+      <c r="H75" s="11">
         <v>18462.3</v>
       </c>
-      <c r="I75" s="12">
+      <c r="I75" s="11">
         <v>2988.1</v>
       </c>
-      <c r="J75" s="12">
+      <c r="J75" s="11">
         <v>4207.2</v>
       </c>
-      <c r="K75" s="12">
+      <c r="K75" s="11">
         <v>12591</v>
       </c>
       <c r="L75" s="5">
@@ -5536,7 +5536,7 @@
       <c r="V75" s="5">
         <v>5607.4</v>
       </c>
-      <c r="W75" s="11"/>
+      <c r="W75" s="10"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -5544,33 +5544,33 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="12">
+        <v>86</v>
+      </c>
+      <c r="C76" s="11">
         <v>32.1</v>
       </c>
-      <c r="D76" s="12">
+      <c r="D76" s="11">
         <v>10.7</v>
       </c>
-      <c r="E76" s="12">
+      <c r="E76" s="11">
         <v>12.4</v>
       </c>
-      <c r="F76" s="12">
+      <c r="F76" s="11">
         <v>53.3</v>
       </c>
-      <c r="G76" s="12">
+      <c r="G76" s="11">
         <v>13.8</v>
       </c>
-      <c r="H76" s="12">
+      <c r="H76" s="11">
         <v>3.3</v>
       </c>
-      <c r="I76" s="12">
+      <c r="I76" s="11">
         <v>20.100000000000001</v>
       </c>
-      <c r="J76" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K76" s="12">
+      <c r="J76" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K76" s="11">
         <v>5.3</v>
       </c>
       <c r="L76" s="5">
@@ -5606,7 +5606,7 @@
       <c r="V76" s="5">
         <v>14.7</v>
       </c>
-      <c r="W76" s="11"/>
+      <c r="W76" s="10"/>
       <c r="X76" s="3"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
@@ -5615,17 +5615,17 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
       <c r="L77" s="5"/>
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
@@ -5637,7 +5637,7 @@
       <c r="T77" s="5"/>
       <c r="U77" s="5"/>
       <c r="V77" s="5"/>
-      <c r="W77" s="11"/>
+      <c r="W77" s="10"/>
       <c r="X77" s="3"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
@@ -5646,33 +5646,33 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
-      </c>
-      <c r="C78" s="12">
+        <v>75</v>
+      </c>
+      <c r="C78" s="11">
         <v>9</v>
       </c>
-      <c r="D78" s="12">
+      <c r="D78" s="11">
         <v>9.6</v>
       </c>
-      <c r="E78" s="12">
+      <c r="E78" s="11">
         <v>0.7</v>
       </c>
-      <c r="F78" s="12">
+      <c r="F78" s="11">
         <v>50.8</v>
       </c>
-      <c r="G78" s="12">
+      <c r="G78" s="11">
         <v>8.4</v>
       </c>
-      <c r="H78" s="12">
+      <c r="H78" s="11">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I78" s="12">
+      <c r="I78" s="11">
         <v>7.6</v>
       </c>
-      <c r="J78" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K78" s="12">
+      <c r="J78" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K78" s="11">
         <v>5</v>
       </c>
       <c r="L78" s="5">
@@ -5703,12 +5703,12 @@
         <v>11.4</v>
       </c>
       <c r="U78" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V78" s="5">
         <v>13.5</v>
       </c>
-      <c r="W78" s="11"/>
+      <c r="W78" s="10"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
@@ -5716,33 +5716,33 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
-      </c>
-      <c r="C79" s="12">
+        <v>87</v>
+      </c>
+      <c r="C79" s="11">
         <v>18.2</v>
       </c>
-      <c r="D79" s="12">
+      <c r="D79" s="11">
         <v>0.6</v>
       </c>
-      <c r="E79" s="12">
+      <c r="E79" s="11">
         <v>1.4</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G79" s="12">
+      <c r="F79" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G79" s="11">
         <v>2.4</v>
       </c>
-      <c r="H79" s="12">
+      <c r="H79" s="11">
         <v>0.8</v>
       </c>
-      <c r="I79" s="12">
+      <c r="I79" s="11">
         <v>9.9</v>
       </c>
-      <c r="J79" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K79" s="12">
+      <c r="J79" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K79" s="11">
         <v>0.3</v>
       </c>
       <c r="L79" s="5">
@@ -5778,12 +5778,12 @@
       <c r="V79" s="5">
         <v>0.6</v>
       </c>
-      <c r="W79" s="11"/>
+      <c r="W79" s="10"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W80" s="6"/>
     </row>

</xml_diff>